<commit_message>
End of Day 6/17     Also removed from cache LinuxTips file put in other dir that is ignored
</commit_message>
<xml_diff>
--- a/pentaho_job_tests_9x.xlsx
+++ b/pentaho_job_tests_9x.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\nod_bts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4201974-C7A6-4B00-80E9-7AEB3B197264}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A6E073A-4B5D-49E5-89A1-D7FBBE096DFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{74926F18-4AF7-4236-B248-DB648E3B46B8}"/>
   </bookViews>
@@ -1242,8 +1242,8 @@
   <sheetPr codeName="Sheet1" filterMode="1"/>
   <dimension ref="A1:L77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B81" sqref="B81"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1258,12 +1258,12 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.4">
       <c r="I1" cm="1">
-        <f t="array" ref="I1">SUMPRODUCT(--(I3:I80=1))/(SUMPRODUCT(--(I3:I80&lt;&gt;1))+SUMPRODUCT(--(I3:I80=1)))</f>
-        <v>0.89743589743589747</v>
+        <f t="array" ref="I1">SUMPRODUCT(--(I3:I78=1))/(SUMPRODUCT(--(I3:I78=0))+SUMPRODUCT(--(I3:I78=1)))</f>
+        <v>0.96052631578947367</v>
       </c>
       <c r="J1" cm="1">
-        <f t="array" ref="J1">SUMPRODUCT(--(J3:J80=1))/(SUMPRODUCT(--(J3:J80&lt;&gt;1))+SUMPRODUCT(--(J3:J80=1)))</f>
-        <v>0.89743589743589747</v>
+        <f t="array" ref="J1">SUMPRODUCT(--(J3:J78=1))/(SUMPRODUCT(--(J3:J78=0))+SUMPRODUCT(--(J3:J78=1)))</f>
+        <v>0.96052631578947367</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="32.15" x14ac:dyDescent="0.4">
@@ -1544,7 +1544,9 @@
       <c r="I9" s="3">
         <v>0</v>
       </c>
-      <c r="J9" s="3"/>
+      <c r="J9" s="3">
+        <v>0</v>
+      </c>
       <c r="K9" s="9" t="s">
         <v>229</v>
       </c>
@@ -3407,8 +3409,12 @@
       <c r="H62" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I62" s="5"/>
-      <c r="J62" s="5"/>
+      <c r="I62" s="5">
+        <v>0</v>
+      </c>
+      <c r="J62" s="5">
+        <v>0</v>
+      </c>
       <c r="K62" s="7" t="s">
         <v>241</v>
       </c>
@@ -3518,7 +3524,7 @@
       <c r="K65" s="9"/>
       <c r="L65" s="9"/>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:12" hidden="1" x14ac:dyDescent="0.4">
       <c r="A66" s="5" t="s">
         <v>180</v>
       </c>
@@ -3543,14 +3549,18 @@
       <c r="H66" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I66" s="5"/>
-      <c r="J66" s="5"/>
+      <c r="I66" s="5">
+        <v>1</v>
+      </c>
+      <c r="J66" s="5">
+        <v>1</v>
+      </c>
       <c r="K66" s="7"/>
       <c r="L66" s="7" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:12" hidden="1" x14ac:dyDescent="0.4">
       <c r="A67" s="3" t="s">
         <v>184</v>
       </c>
@@ -3575,8 +3585,12 @@
       <c r="H67" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I67" s="3"/>
-      <c r="J67" s="3"/>
+      <c r="I67" s="3">
+        <v>1</v>
+      </c>
+      <c r="J67" s="3">
+        <v>1</v>
+      </c>
       <c r="K67" s="9"/>
       <c r="L67" s="9" t="s">
         <v>223</v>
@@ -3792,7 +3806,7 @@
       <c r="K73" s="9"/>
       <c r="L73" s="9"/>
     </row>
-    <row r="74" spans="1:12" ht="20.6" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:12" ht="20.6" hidden="1" x14ac:dyDescent="0.4">
       <c r="A74" s="5" t="s">
         <v>205</v>
       </c>
@@ -3818,9 +3832,11 @@
         <v>6</v>
       </c>
       <c r="I74" s="5">
-        <v>0</v>
-      </c>
-      <c r="J74" s="5"/>
+        <v>1</v>
+      </c>
+      <c r="J74" s="5">
+        <v>1</v>
+      </c>
       <c r="K74" s="7" t="s">
         <v>239</v>
       </c>
@@ -3933,7 +3949,9 @@
   </sheetData>
   <autoFilter ref="A2:K77" xr:uid="{E5343186-B81A-46C5-836C-8FB39BF07858}">
     <filterColumn colId="9">
-      <filters blank="1"/>
+      <filters>
+        <filter val="0"/>
+      </filters>
     </filterColumn>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>